<commit_message>
modified:   CSS Lab Assignment.xlsx
</commit_message>
<xml_diff>
--- a/Pokemon_Site/CSS Lab Assignment.xlsx
+++ b/Pokemon_Site/CSS Lab Assignment.xlsx
@@ -52,28 +52,28 @@
     <t>Adjust the navigation links so that when the cursor hovers over one, it becomes Blue text on a Yellow background.</t>
   </si>
   <si>
-    <t>Create a pseudoclass called logo, and make it so that anything joining that class displays as a block, is centered, and takes up 80% of the available width.</t>
+    <t>Create a pseudoclass called logo, and make it so that anything joining that class displays as a block, and takes up 100% of the width. Also, make any images in that claas display as a block, are centered, and take up 80% of the available width.</t>
   </si>
   <si>
-    <t>Make the index page have a black background, the red page have a light red background, the blue page a light blue background, the yellow page light yellow, and the author page whatyever you want.</t>
+    <t>Make the index page have a black background, the red page have a light red background (hex code #ffcccb), the blue page a light blue background, the yellow page light yellow, the green page light green and the author page whatever you want.</t>
   </si>
   <si>
     <t>Give the index page white text, the "color" pages black text, and the author page whatever you want.</t>
   </si>
   <si>
-    <t>On the index page, make a pseudoclass called content, and make it memberrs of that class are displayed as a block, and H1 headings get a right margin of 10 pixels, and paragraphs have right margins of 20 and left margins of 5 pixels.</t>
+    <t>Make a pseudoclass for the site called content, that displays as a block, floats to the left, and takes up 60% of the available width.  Also create a psuedoclass called sidear that displays as a block, floats right, takes up 39% of the width, displays as a block, floats right, and has a one-pixel solid border along the left side. Each of the pages have Divs labelled CONTENT and SIDEBAR. Join those to the appropriate class.</t>
   </si>
   <si>
-    <t>Create another pseudoclass called sidebar for the index page. this class will be used to display the game images. display the class as a block, float it to the right, and make sure it only fills 33% of the page width.</t>
+    <t>We still need to format the inline elements of the pseudoclasses. So for content, display &lt;h1&gt; headings as blocks, and set the left margin to 5 pixels, &lt;h3&gt; the same, but a 10 pixel margin, and any &lt;p&gt; elements to display as blocks, have a left margin of 15 pixels, and take up 90% of the width of the class. Set a rule to set ANY elements of the sidebar pseudoclass to display as blocks, and only take up 90% of the sidebar width.</t>
   </si>
   <si>
-    <t>Make it so that any images that are in the sidebar are displayed as blocks, and only take up 90% of the width</t>
+    <t>The footer elements still don't display properly. They get moved around by the floating elements. To fix that, create a footer pseudoclass, and use the clear property, setting it to "both". find the footer sections in the HTML files and join those to the class.</t>
   </si>
   <si>
-    <t>Each of the "color pages contains a list of unique aspects of that version. Find the proper place to define a pseudoclass called unique, that floats that list to the right, displays as a block, only takes up 40% of the width, and has a 3 pixel solid black border around the whole piece, not just the list. (the heading and text too)</t>
+    <t>The sidebar on the index page is really too big. Override the width settings in the index style sheet, but let the other settings "cascade" through from the site file. set the content width to 85%, and the sidebar to 14%, to accomodate the border, which should be changed so the color is white.</t>
   </si>
   <si>
-    <t xml:space="preserve">Each of the "color" pages has an image of a game cover. make that "dule" also a member of the unique class, then add the properdefinition so that any image in the class is centered, and takes up only 85% of the width of the class. </t>
+    <t>In order to unify the pages a little more, and to make the Pokemon logo a little flashier, add an id to each style page called #grad. each should be a style that sets the background image to a linear gradient that goes from the base page color, to white, and then back to the base color. (like (black, white, black) for the index page). Then, give each Header div an id of grad.</t>
   </si>
   <si>
     <t>Edit each HTML page so that whichever navigation link matches itself (i.e. the "Home" link on the index page, and the "Red" link on the red page, etc.) is given an id of "current" then create a single css definition that will affect all the pages so that any item inside a nav element with an id of "current" will have an underline.</t>
@@ -89,13 +89,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -110,8 +115,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <fgColor rgb="FFB7B7B7"/>
+        <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,11 +184,11 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -643,7 +648,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="2">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -667,7 +672,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="2">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="D20" s="6"/>
     </row>

</xml_diff>